<commit_message>
unit conv and sankey
</commit_message>
<xml_diff>
--- a/LMADefs-Demo_sl.xlsx
+++ b/LMADefs-Demo_sl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\DemoModels_SelfLearning\DemoS_001_SL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D5974-CA33-4B3F-9F01-12CF8AEE95B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DA91CD-4181-47AB-B091-E4156F7FA496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Unit</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Production/Import</t>
+  </si>
+  <si>
+    <t>NRG,DEM</t>
   </si>
 </sst>
 </file>
@@ -9993,7 +9996,7 @@
   <dimension ref="A2:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10109,7 +10112,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -10141,8 +10144,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>8</v>
+      <c r="G5" s="1" t="str">
+        <f>G4</f>
+        <v>NRG,DEM</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>

</xml_diff>